<commit_message>
alle daten von Google Maps bekommen wurden
</commit_message>
<xml_diff>
--- a/Klinikliste.xlsx
+++ b/Klinikliste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taner/Desktop/klinify/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F2F4CA-3197-CD41-B434-2BFBD7987831}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D77FC1-3B48-2345-B7CF-FF5ABFFB8437}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{CDF4C74C-E155-4ED1-AEE6-0547478CE71C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{CDF4C74C-E155-4ED1-AEE6-0547478CE71C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Klinikname</t>
   </si>
@@ -169,87 +169,6 @@
   </si>
   <si>
     <t>Helios Klinikum Hildesheim</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/AGAPLESION+EV.+KLINIKUM+SCHAUMBURG+gGmbH/@52.2648061,9.1052392,15z/data=!4m2!3m1!1s0x0:0xbb35614cf4b2be1?sa=X&amp;ved=2ahUKEwiV0oq18PDuAhWPO-wKHca5CmoQ_BIwCnoECBcQBQ</t>
-  </si>
-  <si>
-    <t>https://www.klinikbewertungen.de/klinik-forum/erfahrung-mit-krankenhaus-bethel-bueckeburg</t>
-  </si>
-  <si>
-    <t>AGAPLESION EV. KLINIKUM SCHAUMBURG</t>
-  </si>
-  <si>
-    <t>https://www.klinikbewertungen.de/klinik-forum/erfahrung-mit-stadtkrankenhaus-cuxhaven</t>
-  </si>
-  <si>
-    <t>Helios Klinikum Cuxhaven</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/HELIOS+Klinik+Cuxhaven/@53.8528608,8.6921898,15z/data=!4m2!3m1!1s0x0:0x3a2fe1f38b90ded1?sa=X&amp;ved=2ahUKEwjA0ofu8PDuAhVCPuwKHV3mAX0Q_BIwCnoECBkQBQ</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/OsteMed+Klinik+Bremerv%C3%B6rde/@53.47135,9.13539,15z/data=!4m2!3m1!1s0x0:0x9e67a0479524aff6?sa=X&amp;ved=2ahUKEwjbvs7z8fDuAhXaOewKHb8_C-cQ_BIwDXoECBgQBQ</t>
-  </si>
-  <si>
-    <t>https://www.klinikbewertungen.de/klinik-forum/erfahrung-mit-krankenhaus-bremervoerde</t>
-  </si>
-  <si>
-    <t>OsteMed Klinik Bremervörde</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Klinik+Fallingbostel/@52.86903,9.7059601,15z/data=!4m2!3m1!1s0x0:0xdc98c5fc80626f15?sa=X&amp;ved=2ahUKEwiYmdaV8vDuAhWCHewKHabKBksQ_BIwE3oECB8QBQ</t>
-  </si>
-  <si>
-    <t>https://www.klinikbewertungen.de/klinik-forum/erfahrung-mit-klinik-fallingbostel</t>
-  </si>
-  <si>
-    <t>Klinik Fallingborstel</t>
-  </si>
-  <si>
-    <t>https://www.klinikbewertungen.de/klinik-forum/erfahrung-mit-klinikum-emden</t>
-  </si>
-  <si>
-    <t>Klinikum Emden</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Klinikum+Emden+-+Hans-Susemihl-Krankenhaus/@53.3754445,7.2129241,15z/data=!4m2!3m1!1s0x0:0x5db7edd86596419e?sa=X&amp;ved=2ahUKEwiDpfyV9PDuAhWCjaQKHWgBCcwQ_BIwD3oECCMQBQ</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Krankenhaus+Ludmillenstift/@52.688896,7.2928619,15z/data=!4m2!3m1!1s0x0:0x59c2048e1a4953f?sa=X&amp;ved=2ahUKEwigpYag9vDuAhWxwAIHHXwPDugQ_BIwDXoECBYQBQ</t>
-  </si>
-  <si>
-    <t>https://www.klinikbewertungen.de/klinik-forum/erfahrung-mit-krankenhaus-ludmillenstift-meppen</t>
-  </si>
-  <si>
-    <t>Krankenhaus Ludmillenstift</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Marienkrankenhaus+Papenburg-+Aschendorf+GmbH+Betriebsst%C3%A4tte+Aschendorf/@53.05092,7.3292999,15z/data=!4m5!3m4!1s0x0:0x20891ebe2b01a054!8m2!3d53.05092!4d7.3292999</t>
-  </si>
-  <si>
-    <t>https://www.klinikbewertungen.de/klinik-forum/erfahrung-mit-marienhospital-papenburg</t>
-  </si>
-  <si>
-    <t>Marienhospital Papenburg</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Kreiskrankenhaus+Osterholz/@53.2337217,8.7942051,15z/data=!4m2!3m1!1s0x0:0xee4b35384cb3b2ad?sa=X&amp;ved=2ahUKEwjYrbHu8fDuAhVRyaQKHSREAa0Q_BIwDXoECBYQBQ</t>
-  </si>
-  <si>
-    <t>Kreiskrankenhaus Osterholz</t>
-  </si>
-  <si>
-    <t>https://www.klinikbewertungen.de/klinik-forum/erfahrung-mit-krankenhaus-osterholz-scharmbeck</t>
-  </si>
-  <si>
-    <t>https://www.klinikbewertungen.de/klinik-forum/erfahrung-mit-krankenhaus-soltau</t>
-  </si>
-  <si>
-    <t>Krankenhaus Soltau</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Heidekreis-Klinikum+GmbH+Krankenhaus+Soltau/@52.9894409,9.847291,15z/data=!3m1!4b1!4m8!1m2!11m1!2s1tsS4C8icZfBtXgqho9ekuv3aB34!3m4!1s0x47b1b</t>
   </si>
 </sst>
 </file>
@@ -316,8 +235,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22FD3C9B-50FA-4678-BE53-0EE801DE3D8A}" name="Tabelle1" displayName="Tabelle1" ref="A1:C35" totalsRowShown="0">
-  <autoFilter ref="A1:C35" xr:uid="{93FFACCF-88EC-40DD-8F5C-DAF85EAF4E94}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22FD3C9B-50FA-4678-BE53-0EE801DE3D8A}" name="Tabelle1" displayName="Tabelle1" ref="A1:C16" totalsRowShown="0">
+  <autoFilter ref="A1:C16" xr:uid="{93FFACCF-88EC-40DD-8F5C-DAF85EAF4E94}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E451B32B-8D07-436F-BE4A-9B074A899C73}" name="Klinikname"/>
     <tableColumn id="2" xr3:uid="{0D47BC81-6708-4D65-A7C1-CF72DBD4A249}" name="Link Google Maps"/>
@@ -624,7 +543,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3474B27-FD20-4EE7-B036-C220E6D6A0ED}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
@@ -812,145 +731,6 @@
       <c r="C16" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>73</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -980,24 +760,11 @@
     <hyperlink ref="C15" r:id="rId24" xr:uid="{9CC89BA9-F6FE-4AAD-969B-3AB82FEE3758}"/>
     <hyperlink ref="C16" r:id="rId25" xr:uid="{B7D7089A-010F-412E-9A71-CB1F89D0F630}"/>
     <hyperlink ref="B16" r:id="rId26" xr:uid="{D24417EB-471C-48C7-86E7-88583346EF47}"/>
-    <hyperlink ref="B17" r:id="rId27" xr:uid="{AEF1DD6A-1E71-4156-BD5E-368D3D7C72AA}"/>
-    <hyperlink ref="B18" r:id="rId28" xr:uid="{AE308C15-E685-462C-B24C-7E333366EEBF}"/>
-    <hyperlink ref="B20" r:id="rId29" xr:uid="{227ABD92-F083-47CE-A1E1-3290D04B844C}"/>
-    <hyperlink ref="C20" r:id="rId30" xr:uid="{1BDD6D14-DD66-4712-8535-8C1C75D74396}"/>
-    <hyperlink ref="C21" r:id="rId31" xr:uid="{39619E61-4182-4C1A-8F99-DE35D6464743}"/>
-    <hyperlink ref="B21" r:id="rId32" xr:uid="{3FE4B2F7-4B09-451C-AB70-7341FED620E0}"/>
-    <hyperlink ref="B22" r:id="rId33" xr:uid="{E34C8FC4-70AE-4938-97E6-15310D471AA5}"/>
-    <hyperlink ref="C22" r:id="rId34" xr:uid="{544D306D-1139-4BFD-A971-28DB5F2888C4}"/>
-    <hyperlink ref="B23" r:id="rId35" xr:uid="{372F342C-AEC7-4046-9363-FD723391A27C}"/>
-    <hyperlink ref="B24" r:id="rId36" xr:uid="{F47C5E1A-4057-4AC5-93C3-7FEB4B58C626}"/>
-    <hyperlink ref="C24" r:id="rId37" xr:uid="{2874C5E4-D958-4DC3-9EB9-31FC92022333}"/>
-    <hyperlink ref="C25" r:id="rId38" xr:uid="{1004405F-E09A-4241-B110-4D6DFF97D342}"/>
-    <hyperlink ref="B25" r:id="rId39" xr:uid="{76406749-A023-7A4D-B392-7A6B50AF22C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId40"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId27"/>
   <tableParts count="1">
-    <tablePart r:id="rId41"/>
+    <tablePart r:id="rId28"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>